<commit_message>
fixed some more bugs
</commit_message>
<xml_diff>
--- a/tests/testMaterials/cdsTestData/CDSSparse_2020_2021.xlsx
+++ b/tests/testMaterials/cdsTestData/CDSSparse_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\tests\testMaterials\cdsTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D616AAE8-F7F2-4EDE-AFA8-B80328D2402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C78AC8-AF36-4B99-AED2-65C3339CACAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_general" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="344">
   <si>
     <t>Value</t>
   </si>
@@ -164,15 +164,9 @@
     <t>hispanic</t>
   </si>
   <si>
-    <t>african americans</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
-    <t>american indians</t>
-  </si>
-  <si>
     <t>asian</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
   </si>
   <si>
     <t>How many degree-seeking first-time first-year students are enrolled?</t>
-  </si>
-  <si>
-    <t>first-year american indians</t>
   </si>
   <si>
     <t>36</t>
@@ -1072,6 +1063,12 @@
   </si>
   <si>
     <t>The type of college-owned, -operated, or -affiliated housing available include the following: coed dorms, men's dorms, apartment for single students, fraternity/sorority housing, and theme housing</t>
+  </si>
+  <si>
+    <t>american indian</t>
+  </si>
+  <si>
+    <t>african american</t>
   </si>
 </sst>
 </file>
@@ -3927,46 +3924,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -3989,7 +3986,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4054,7 +4051,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4119,7 +4116,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4184,7 +4181,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4249,7 +4246,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4314,7 +4311,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4785,49 +4782,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>17</v>
@@ -4850,7 +4847,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4918,7 +4915,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4986,7 +4983,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5054,7 +5051,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5122,7 +5119,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5190,7 +5187,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5258,7 +5255,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5326,7 +5323,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5394,7 +5391,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5462,7 +5459,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5530,7 +5527,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5598,7 +5595,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6090,61 +6087,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -6167,7 +6164,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6247,7 +6244,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6327,7 +6324,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6407,7 +6404,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6487,7 +6484,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6567,7 +6564,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6647,7 +6644,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6727,7 +6724,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6807,7 +6804,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6887,7 +6884,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6967,7 +6964,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -7543,28 +7540,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -7587,7 +7584,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7634,7 +7631,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7681,7 +7678,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7728,7 +7725,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -7775,7 +7772,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7822,7 +7819,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -8177,67 +8174,67 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>26</v>
@@ -8246,28 +8243,28 @@
         <v>1</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>17</v>
@@ -8287,7 +8284,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8403,7 +8400,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -8519,7 +8516,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -8635,7 +8632,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8751,7 +8748,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8867,7 +8864,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -8983,7 +8980,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9099,7 +9096,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9215,7 +9212,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -9331,7 +9328,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -9447,7 +9444,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -9563,7 +9560,7 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -9679,7 +9676,7 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -9795,7 +9792,7 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -9911,7 +9908,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -10027,7 +10024,7 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -10143,7 +10140,7 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -10259,7 +10256,7 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -10375,7 +10372,7 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -10491,7 +10488,7 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -10607,7 +10604,7 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -11322,10 +11319,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -11354,7 +11351,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -11392,7 +11389,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -11468,7 +11465,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -11506,7 +11503,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -11828,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -11849,61 +11846,61 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>17</v>
@@ -11923,7 +11920,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12021,7 +12018,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -12119,7 +12116,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -12217,7 +12214,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -12315,7 +12312,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -12413,7 +12410,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -12511,7 +12508,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -12609,7 +12606,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -12707,7 +12704,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -12805,7 +12802,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -12903,7 +12900,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -13001,7 +12998,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -13099,7 +13096,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -13197,7 +13194,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -13295,7 +13292,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -13393,7 +13390,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -13999,40 +13996,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>17</v>
@@ -14052,7 +14049,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -14108,7 +14105,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -14164,7 +14161,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -14220,7 +14217,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -14276,7 +14273,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -14619,9 +14616,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -14646,31 +14653,31 @@
         <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>17</v>
@@ -14691,12 +14698,12 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -14767,7 +14774,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -14838,7 +14845,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -14909,7 +14916,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -15051,7 +15058,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -15193,7 +15200,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -15264,7 +15271,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -15761,7 +15768,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -15840,12 +15847,15 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" customWidth="1"/>
+    <col min="12" max="12" width="40.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -15877,31 +15887,31 @@
         <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>17</v>
@@ -15922,12 +15932,12 @@
         <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16004,7 +16014,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16081,7 +16091,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -16158,7 +16168,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -16312,7 +16322,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -16466,7 +16476,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -17082,7 +17092,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -17181,79 +17191,79 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>17</v>
@@ -17276,7 +17286,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -17374,7 +17384,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -17472,7 +17482,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -17864,7 +17874,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -17962,7 +17972,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -18060,7 +18070,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -18158,7 +18168,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -18256,7 +18266,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -18354,7 +18364,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -18452,7 +18462,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -18648,7 +18658,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -19040,7 +19050,7 @@
     </row>
     <row r="20" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -19138,7 +19148,7 @@
     </row>
     <row r="21" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -19645,61 +19655,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -19707,7 +19717,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -19772,7 +19782,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -19837,7 +19847,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -19902,7 +19912,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -19967,7 +19977,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -20032,7 +20042,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -20097,7 +20107,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -20162,7 +20172,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -20227,7 +20237,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -20292,7 +20302,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -20357,7 +20367,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -20422,7 +20432,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -20487,7 +20497,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -20552,7 +20562,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -20617,7 +20627,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -20682,7 +20692,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -20747,7 +20757,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -20812,7 +20822,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -20877,7 +20887,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -20942,7 +20952,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -21023,69 +21033,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -21150,7 +21160,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -21215,7 +21225,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -21280,7 +21290,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -21345,7 +21355,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -21410,7 +21420,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -21475,7 +21485,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -21540,7 +21550,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -21605,7 +21615,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -21670,7 +21680,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -21735,7 +21745,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -21807,7 +21817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -21823,46 +21833,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -21885,7 +21895,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -21950,7 +21960,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -22015,7 +22025,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -22080,7 +22090,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -22145,7 +22155,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -22210,7 +22220,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -22275,7 +22285,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -22340,7 +22350,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -22405,7 +22415,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -22470,7 +22480,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -22535,7 +22545,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -22600,7 +22610,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -22665,7 +22675,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -22730,7 +22740,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -22795,7 +22805,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -22860,7 +22870,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -22925,7 +22935,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -22990,7 +23000,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -23055,7 +23065,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -23120,7 +23130,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -23185,7 +23195,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -23250,7 +23260,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -23315,7 +23325,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -23380,7 +23390,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -23445,7 +23455,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -23510,7 +23520,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -23575,7 +23585,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -23640,7 +23650,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -23705,7 +23715,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -23770,7 +23780,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -23835,7 +23845,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -23900,7 +23910,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -23965,7 +23975,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -24030,7 +24040,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -24095,7 +24105,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -24160,7 +24170,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -24631,52 +24641,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
@@ -24699,7 +24709,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -24770,7 +24780,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -24841,7 +24851,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -24912,7 +24922,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -24983,7 +24993,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -25054,7 +25064,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -25569,58 +25579,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
@@ -25643,7 +25653,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -25720,7 +25730,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -25797,7 +25807,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -25874,7 +25884,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -25951,7 +25961,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -26028,7 +26038,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -26105,7 +26115,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -26182,7 +26192,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -26259,7 +26269,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -26336,7 +26346,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -26413,7 +26423,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -26490,7 +26500,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>